<commit_message>
EURUSD New Table, Graph Upload
- Added a new table in the excel
- Saved the image of the graph
</commit_message>
<xml_diff>
--- a/Trading_Performance_Metrics.xlsx
+++ b/Trading_Performance_Metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Avaneesh\Desktop\MachineLearningProject\Volatility-Forecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F01EA8A-BD2F-4F33-9CEC-4286FFFFA07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E85603-F998-406A-9AA9-7C31F93CD7BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{6773E164-2547-456B-A28E-7CA37EE73E78}"/>
   </bookViews>
@@ -144,13 +144,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1161,13 +1162,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3B1CA9-DA7A-4A26-8732-B3CA92318318}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.4">
@@ -1197,87 +1202,207 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="B2" s="6">
+        <v>1.2467000000000001E-2</v>
+      </c>
+      <c r="C2" s="6">
+        <v>8.2794999999999994E-2</v>
+      </c>
+      <c r="D2">
+        <v>0.15767500000000001</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.15055789999999999</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1.1906E-2</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.24171500000000001</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="B3" s="6">
+        <v>-9.6311999999999995E-2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>9.8265000000000005E-2</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.21096899999999999</v>
+      </c>
+      <c r="E3" s="6">
+        <v>-0.98012900000000003</v>
+      </c>
+      <c r="F3" s="6">
+        <v>-0.44745200000000002</v>
+      </c>
+      <c r="G3" s="6">
+        <v>-1.445568</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="B4" s="6">
+        <v>-9.6311999999999995E-2</v>
+      </c>
+      <c r="C4" s="6">
+        <v>9.8265000000000005E-2</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.21096899999999999</v>
+      </c>
+      <c r="E4" s="6">
+        <v>-0.98012900000000003</v>
+      </c>
+      <c r="F4" s="6">
+        <v>-0.44745200000000002</v>
+      </c>
+      <c r="G4" s="6">
+        <v>-1.445568</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="B5" s="6">
+        <v>6.7321000000000006E-2</v>
+      </c>
+      <c r="C5" s="6">
+        <v>7.4702000000000005E-2</v>
+      </c>
+      <c r="D5" s="6">
+        <v>6.4708000000000002E-2</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.90118500000000001</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.95229399999999997</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1.226135</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="B6" s="6">
+        <v>4.8557000000000003E-2</v>
+      </c>
+      <c r="C6" s="6">
+        <v>8.2657999999999995E-2</v>
+      </c>
+      <c r="D6" s="6">
+        <v>8.0129000000000006E-2</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.58744600000000002</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.35598200000000002</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.92338699999999996</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="B7" s="6">
+        <v>2.0188999999999999E-2</v>
+      </c>
+      <c r="C7" s="6">
+        <v>8.2707000000000003E-2</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.13387299999999999</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0.24410899999999999</v>
+      </c>
+      <c r="F7" s="6">
+        <v>3.6814E-2</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0.417182</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="B8" s="6">
+        <v>2.9374999999999998E-2</v>
+      </c>
+      <c r="C8" s="6">
+        <v>9.9538000000000001E-2</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.13387299999999999</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.29510999999999998</v>
+      </c>
+      <c r="F8" s="6">
+        <v>6.4753000000000005E-2</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.50434299999999999</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B9" s="6">
+        <v>-3.7469000000000002E-2</v>
+      </c>
+      <c r="C9" s="6">
+        <v>4.6461000000000002E-2</v>
+      </c>
+      <c r="D9" s="6">
+        <v>4.0779000000000003E-2</v>
+      </c>
+      <c r="E9" s="6">
+        <v>-0.80647100000000005</v>
+      </c>
+      <c r="F9" s="6">
+        <v>-0.74101600000000001</v>
+      </c>
+      <c r="G9" s="6">
+        <v>-0.97411400000000004</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="B10" s="6">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="C10" s="6">
+        <v>5.645E-2</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.12023399999999999</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.90345500000000001</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.38322200000000001</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1.2857670000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>